<commit_message>
Changed CPI to PCE
</commit_message>
<xml_diff>
--- a/Descriptive statistics.xlsx
+++ b/Descriptive statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptives of Yields (Ortec)" sheetId="1" r:id="rId1"/>
@@ -192,8 +192,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -231,6 +235,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -240,6 +246,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2829,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="A1:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,7 +3111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3502,5 +3512,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>